<commit_message>
added transmission sign definitions
</commit_message>
<xml_diff>
--- a/tables/Dataset S1.xlsx
+++ b/tables/Dataset S1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mike/Documents/GitHub/SCTLD-sediment-transmission/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.studivan/Documents/GitHub/SCTLD-sediment-transmission/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14D3FCBB-F5FA-4E48-B46E-86F2D2480C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1533C4-6A68-A043-9ADF-9D496481CD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2360" windowWidth="27640" windowHeight="16940" xr2:uid="{54F47576-6138-E241-946F-DE6C6338C18C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="122">
   <si>
     <t>Sample ID</t>
   </si>
@@ -361,6 +361,45 @@
   </si>
   <si>
     <t xml:space="preserve">0 days 21 hrs 30 mins </t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>Mesenterial filaments</t>
+  </si>
+  <si>
+    <t>Mucus</t>
+  </si>
+  <si>
+    <t>Mucus production</t>
+  </si>
+  <si>
+    <t>Necrosis</t>
+  </si>
+  <si>
+    <t>Liquefactive necrosis</t>
+  </si>
+  <si>
+    <t>Paling</t>
+  </si>
+  <si>
+    <t>Tissue paling/bleaching</t>
+  </si>
+  <si>
+    <t>Swelling</t>
+  </si>
+  <si>
+    <t>Tissue swelling</t>
+  </si>
+  <si>
+    <t>Tissue loss</t>
   </si>
 </sst>
 </file>
@@ -427,7 +466,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -455,11 +494,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -507,6 +555,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -823,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FC3FAA-942B-094D-B8E2-1D01B4EFA909}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2611,7 +2677,87 @@
         <v>0.89583333333333337</v>
       </c>
     </row>
+    <row r="62" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+    </row>
+    <row r="64" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+    </row>
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>